<commit_message>
Update KRI Liver Segmentation Evaluation v2.xlsx
</commit_message>
<xml_diff>
--- a/kri-evaluation/results/KRI Liver Segmentation Evaluation v2.xlsx
+++ b/kri-evaluation/results/KRI Liver Segmentation Evaluation v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Master thesis\master\kri-evaluation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0472973F-450D-47C3-ADA6-099D6095DC2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0F01AB-AF2B-4EA8-9238-D53D8A9537A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kri" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="kri-nn-postpr" sheetId="5" r:id="rId3"/>
     <sheet name="raw" sheetId="4" r:id="rId4"/>
     <sheet name="etc" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">kri!$A$1:$F$104</definedName>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -317,9 +316,6 @@
   </si>
   <si>
     <t>???</t>
-  </si>
-  <si>
-    <t>28.05.2020</t>
   </si>
   <si>
     <t>This is the volumetry computed by the nn without supervision removing all islands in the generated prediction, with morphological operations conect islands tat aver very close.
@@ -832,7 +828,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1035,7 +1031,6 @@
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1069,6 +1064,27 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1092,27 +1108,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6100,10 +6095,10 @@
       <c r="P4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="92" t="s">
+      <c r="R4" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="92"/>
+      <c r="S4" s="83"/>
       <c r="U4" s="27" t="s">
         <v>2</v>
       </c>
@@ -6147,10 +6142,10 @@
         <f>AVERAGEIFS(G2:G104,G2:G104,"&lt;&gt;0",G2:G104,"&lt;50%")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U5" s="83" t="s">
+      <c r="U5" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="80" t="s">
+      <c r="V5" s="86" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6190,8 +6185,8 @@
         <f>STDEV(G2:G104)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U6" s="84"/>
-      <c r="V6" s="81"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="87"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
@@ -6237,8 +6232,8 @@
         <f>AVERAGEIF(H4:H106,"&lt;&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U7" s="84"/>
-      <c r="V7" s="81"/>
+      <c r="U7" s="90"/>
+      <c r="V7" s="87"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
@@ -6280,8 +6275,8 @@
       <c r="P8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="U8" s="84"/>
-      <c r="V8" s="81"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="87"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -6320,12 +6315,12 @@
         <f t="shared" si="0"/>
         <v>7.5711987127916255E-2</v>
       </c>
-      <c r="R9" s="92" t="s">
+      <c r="R9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="S9" s="92"/>
-      <c r="U9" s="86"/>
-      <c r="V9" s="87"/>
+      <c r="S9" s="83"/>
+      <c r="U9" s="92"/>
+      <c r="V9" s="93"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
@@ -6363,10 +6358,10 @@
         <f>AVERAGEIFS(K2:K104,K2:K104,"&lt;&gt;0",K2:K104,"&lt;30%")</f>
         <v>6.3609986190155884E-2</v>
       </c>
-      <c r="U10" s="83" t="s">
+      <c r="U10" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="V10" s="80" t="s">
+      <c r="V10" s="86" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6414,8 +6409,8 @@
         <f>STDEV(K2:K104)</f>
         <v>0.21826631915929956</v>
       </c>
-      <c r="U11" s="84"/>
-      <c r="V11" s="81"/>
+      <c r="U11" s="90"/>
+      <c r="V11" s="87"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
@@ -6461,8 +6456,8 @@
         <f>AVERAGEIF(L4:L106,"&lt;&gt;0")</f>
         <v>0.90393372549019602</v>
       </c>
-      <c r="U12" s="84"/>
-      <c r="V12" s="81"/>
+      <c r="U12" s="90"/>
+      <c r="V12" s="87"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -6495,8 +6490,8 @@
       </c>
       <c r="R13"/>
       <c r="S13"/>
-      <c r="U13" s="84"/>
-      <c r="V13" s="81"/>
+      <c r="U13" s="90"/>
+      <c r="V13" s="87"/>
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
@@ -6535,12 +6530,12 @@
         <f t="shared" si="0"/>
         <v>4.6106438980548205E-2</v>
       </c>
-      <c r="R14" s="93" t="s">
+      <c r="R14" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="S14" s="94"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="87"/>
+      <c r="S14" s="85"/>
+      <c r="U14" s="92"/>
+      <c r="V14" s="93"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
@@ -6578,10 +6573,10 @@
         <f>AVERAGEIFS(O2:O104,O2:O104,"&lt;&gt;0",O2:O104,"&lt;50%")</f>
         <v>0.12434032373984207</v>
       </c>
-      <c r="U15" s="83" t="s">
+      <c r="U15" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="V15" s="80" t="s">
+      <c r="V15" s="86" t="s">
         <v>31</v>
       </c>
     </row>
@@ -6621,8 +6616,8 @@
         <f>STDEV(O2:O104)</f>
         <v>0.14978376778042762</v>
       </c>
-      <c r="U16" s="84"/>
-      <c r="V16" s="81"/>
+      <c r="U16" s="90"/>
+      <c r="V16" s="87"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
@@ -6653,8 +6648,8 @@
         <f t="shared" si="0"/>
         <v>4.5371036467268006E-2</v>
       </c>
-      <c r="U17" s="84"/>
-      <c r="V17" s="81"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="87"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
@@ -6685,8 +6680,8 @@
         <f t="shared" si="0"/>
         <v>0.2329903750414869</v>
       </c>
-      <c r="U18" s="84"/>
-      <c r="V18" s="81"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="87"/>
     </row>
     <row r="19" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24">
@@ -6717,8 +6712,8 @@
         <f t="shared" si="0"/>
         <v>0.26341668729883638</v>
       </c>
-      <c r="U19" s="85"/>
-      <c r="V19" s="82"/>
+      <c r="U19" s="91"/>
+      <c r="V19" s="88"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
@@ -9653,10 +9648,10 @@
       <c r="L106" s="32"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B107" s="88" t="s">
+      <c r="B107" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="C107" s="89"/>
+      <c r="C107" s="80"/>
       <c r="D107" s="47">
         <f>COUNTIF(D2:D104,"=mr")</f>
         <v>55</v>
@@ -9665,10 +9660,10 @@
       <c r="L107" s="32"/>
     </row>
     <row r="108" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="90" t="s">
+      <c r="B108" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="C108" s="91"/>
+      <c r="C108" s="82"/>
       <c r="D108" s="48">
         <f>COUNTIF(D2:D104,"=ct")</f>
         <v>46</v>
@@ -10014,17 +10009,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R14:S14"/>
     <mergeCell ref="V15:V19"/>
     <mergeCell ref="U15:U19"/>
     <mergeCell ref="U5:U9"/>
     <mergeCell ref="V5:V9"/>
     <mergeCell ref="U10:U14"/>
     <mergeCell ref="V10:V14"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R14:S14"/>
   </mergeCells>
   <conditionalFormatting sqref="O2:O104">
     <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
@@ -10050,7 +10045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="S5" sqref="S5"/>
     </sheetView>
@@ -10062,9 +10057,9 @@
     <col min="3" max="3" width="9.5703125" style="37" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="75" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="77" customWidth="1"/>
-    <col min="8" max="8" width="10" style="76" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="74" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="76" customWidth="1"/>
+    <col min="8" max="8" width="10" style="75" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" style="21" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="31" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" style="37" customWidth="1"/>
@@ -10096,13 +10091,13 @@
         <v>4</v>
       </c>
       <c r="E1" s="22"/>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="71" t="s">
         <v>46</v>
       </c>
       <c r="I1" s="22"/>
@@ -10146,14 +10141,14 @@
         <v>ct</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="73">
+      <c r="F2" s="72">
         <v>1487.85</v>
       </c>
-      <c r="G2" s="74">
+      <c r="G2" s="73">
         <f>+ABS((C2-F2)/C2)</f>
         <v>0.10671829971181557</v>
       </c>
-      <c r="H2" s="78">
+      <c r="H2" s="77">
         <v>0.89539999999999997</v>
       </c>
       <c r="I2" s="3"/>
@@ -10185,18 +10180,18 @@
         <v>ct</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="75">
+      <c r="F3" s="74">
         <v>430.29</v>
       </c>
-      <c r="G3" s="74">
+      <c r="G3" s="73">
         <f>+ABS((C3-F3)/C3)</f>
         <v>0.63304622207061234</v>
       </c>
-      <c r="H3" s="78">
+      <c r="H3" s="77">
         <v>0.47183000000000003</v>
       </c>
       <c r="K3" s="49"/>
-      <c r="N3" s="69">
+      <c r="N3" s="68">
         <v>2308.64</v>
       </c>
       <c r="O3" s="61">
@@ -10222,14 +10217,14 @@
         <v>ct</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="75">
+      <c r="F4" s="74">
         <v>2068.66</v>
       </c>
-      <c r="G4" s="74">
+      <c r="G4" s="73">
         <f>+ABS((C4-F4)/C4)</f>
         <v>2.0935841775205719E-3</v>
       </c>
-      <c r="H4" s="78">
+      <c r="H4" s="77">
         <v>0.87870000000000004</v>
       </c>
       <c r="K4" s="49"/>
@@ -10243,14 +10238,14 @@
       <c r="P4" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="92" t="s">
+      <c r="R4" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="92"/>
-      <c r="U4" s="95" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="96"/>
+      <c r="S4" s="83"/>
+      <c r="U4" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4" s="95"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="56">
@@ -10270,14 +10265,14 @@
         <v>ct</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="75">
+      <c r="F5" s="74">
         <v>1813.23</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="73">
         <f>+ABS((C5-F5)/C5)</f>
         <v>8.4705228031145812E-3</v>
       </c>
-      <c r="H5" s="78">
+      <c r="H5" s="77">
         <v>0.92969999999999997</v>
       </c>
       <c r="K5" s="49"/>
@@ -10295,8 +10290,8 @@
         <f>AVERAGEIFS(G2:G104,G2:G104,"&lt;&gt;0",G2:G104,"&lt;30%")</f>
         <v>6.3525422634634648E-2</v>
       </c>
-      <c r="U5" s="97"/>
-      <c r="V5" s="98"/>
+      <c r="U5" s="96"/>
+      <c r="V5" s="97"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="56">
@@ -10316,14 +10311,14 @@
         <v>ct</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="75">
+      <c r="F6" s="74">
         <v>1676.44</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="73">
         <f>+ABS((C6-F6)/C6)</f>
         <v>5.6005405709780971E-2</v>
       </c>
-      <c r="H6" s="78">
+      <c r="H6" s="77">
         <v>0.9073</v>
       </c>
       <c r="K6" s="49"/>
@@ -10341,8 +10336,8 @@
         <f>STDEV(G2:G104)</f>
         <v>0.22863269908852635</v>
       </c>
-      <c r="U6" s="97"/>
-      <c r="V6" s="98"/>
+      <c r="U6" s="96"/>
+      <c r="V6" s="97"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="56">
@@ -10362,8 +10357,8 @@
         <v>mr</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="79"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="78"/>
       <c r="J7" s="31">
         <v>1533.96</v>
       </c>
@@ -10388,8 +10383,8 @@
         <f>AVERAGEIF(H4:H106,"&lt;&gt;0")</f>
         <v>0.86147209302325589</v>
       </c>
-      <c r="U7" s="97"/>
-      <c r="V7" s="98"/>
+      <c r="U7" s="96"/>
+      <c r="V7" s="97"/>
     </row>
     <row r="8" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
@@ -10409,8 +10404,8 @@
         <v>mr</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="79"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="78"/>
       <c r="J8" s="31">
         <v>1512.47</v>
       </c>
@@ -10431,8 +10426,8 @@
       <c r="P8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="U8" s="99"/>
-      <c r="V8" s="100"/>
+      <c r="U8" s="98"/>
+      <c r="V8" s="99"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="56">
@@ -10452,8 +10447,8 @@
         <v>mr</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="79"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="78"/>
       <c r="J9" s="31">
         <v>1277.24</v>
       </c>
@@ -10471,10 +10466,10 @@
         <f t="shared" si="0"/>
         <v>0.15115044247787621</v>
       </c>
-      <c r="R9" s="92" t="s">
+      <c r="R9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="S9" s="92"/>
+      <c r="S9" s="83"/>
       <c r="U9" s="25" t="s">
         <v>1</v>
       </c>
@@ -10500,14 +10495,14 @@
         <v>ct</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="75">
+      <c r="F10" s="74">
         <v>1390.57</v>
       </c>
-      <c r="G10" s="74">
+      <c r="G10" s="73">
         <f t="shared" ref="G10:G69" si="2">+ABS((C10-F10)/C10)</f>
         <v>8.291894743784213E-2</v>
       </c>
-      <c r="H10" s="78"/>
+      <c r="H10" s="77"/>
       <c r="K10" s="49"/>
       <c r="N10" s="60">
         <v>1519.63</v>
@@ -10548,8 +10543,8 @@
         <v>mr</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="79"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="78"/>
       <c r="J11" s="31">
         <v>1338.03</v>
       </c>
@@ -10574,10 +10569,10 @@
         <f>STDEV(K2:K104)</f>
         <v>6.5777584983879742E-2</v>
       </c>
-      <c r="U11" s="83" t="s">
+      <c r="U11" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="V11" s="80" t="s">
+      <c r="V11" s="86" t="s">
         <v>60</v>
       </c>
     </row>
@@ -10599,8 +10594,8 @@
         <v>mr</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="79"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="78"/>
       <c r="J12" s="31">
         <v>1494.06</v>
       </c>
@@ -10625,8 +10620,8 @@
         <f>AVERAGEIF(L4:L106,"&lt;&gt;0")</f>
         <v>0.91582571153846171</v>
       </c>
-      <c r="U12" s="84"/>
-      <c r="V12" s="81"/>
+      <c r="U12" s="90"/>
+      <c r="V12" s="87"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="56">
@@ -10646,14 +10641,14 @@
         <v>ct</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="75">
+      <c r="F13" s="74">
         <v>1374.88</v>
       </c>
-      <c r="G13" s="74">
+      <c r="G13" s="73">
         <f t="shared" si="2"/>
         <v>6.221949389536853E-2</v>
       </c>
-      <c r="H13" s="78">
+      <c r="H13" s="77">
         <v>0.89029999999999998</v>
       </c>
       <c r="K13" s="49"/>
@@ -10666,8 +10661,8 @@
       </c>
       <c r="R13"/>
       <c r="S13"/>
-      <c r="U13" s="84"/>
-      <c r="V13" s="81"/>
+      <c r="U13" s="90"/>
+      <c r="V13" s="87"/>
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56">
@@ -10687,8 +10682,8 @@
         <v>mr</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="79"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="78"/>
       <c r="J14" s="31">
         <v>1700.27</v>
       </c>
@@ -10706,12 +10701,12 @@
         <f t="shared" si="0"/>
         <v>1.9727803813314512E-2</v>
       </c>
-      <c r="R14" s="93" t="s">
+      <c r="R14" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="S14" s="94"/>
-      <c r="U14" s="84"/>
-      <c r="V14" s="81"/>
+      <c r="S14" s="85"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="87"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="56">
@@ -10731,14 +10726,14 @@
         <v>ct</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="75">
+      <c r="F15" s="74">
         <v>1544.65</v>
       </c>
-      <c r="G15" s="74">
+      <c r="G15" s="73">
         <f t="shared" si="2"/>
         <v>0.13290108903109912</v>
       </c>
-      <c r="H15" s="78">
+      <c r="H15" s="77">
         <v>0.91269999999999996</v>
       </c>
       <c r="K15" s="49"/>
@@ -10756,8 +10751,8 @@
         <f>AVERAGEIFS(O2:O104,O2:O104,"&lt;&gt;0",O2:O104,"&lt;50%")</f>
         <v>0.13379201009127831</v>
       </c>
-      <c r="U15" s="86"/>
-      <c r="V15" s="87"/>
+      <c r="U15" s="92"/>
+      <c r="V15" s="93"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="56">
@@ -10777,14 +10772,14 @@
         <v>ct</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="75">
+      <c r="F16" s="74">
         <v>2029.93</v>
       </c>
-      <c r="G16" s="74">
+      <c r="G16" s="73">
         <f t="shared" si="2"/>
         <v>0.10733069481090586</v>
       </c>
-      <c r="H16" s="78">
+      <c r="H16" s="77">
         <v>0.91539999999999999</v>
       </c>
       <c r="K16" s="49"/>
@@ -10802,10 +10797,10 @@
         <f>STDEV(O2:O104)</f>
         <v>0.16965740518188058</v>
       </c>
-      <c r="U16" s="83" t="s">
+      <c r="U16" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="V16" s="80" t="s">
+      <c r="V16" s="86" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10827,14 +10822,14 @@
         <v>ct</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="75">
+      <c r="F17" s="74">
         <v>1818.16</v>
       </c>
-      <c r="G17" s="74">
+      <c r="G17" s="73">
         <f t="shared" si="2"/>
         <v>6.1203032482984743E-3</v>
       </c>
-      <c r="H17" s="78">
+      <c r="H17" s="77">
         <v>0.88680000000000003</v>
       </c>
       <c r="K17" s="49"/>
@@ -10845,8 +10840,8 @@
         <f t="shared" si="0"/>
         <v>4.5985280283326576E-3</v>
       </c>
-      <c r="U17" s="84"/>
-      <c r="V17" s="81"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="87"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="56">
@@ -10866,14 +10861,14 @@
         <v>ct</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="75">
+      <c r="F18" s="74">
         <v>360.16</v>
       </c>
-      <c r="G18" s="74">
+      <c r="G18" s="73">
         <f t="shared" si="2"/>
         <v>0.76092930633919675</v>
       </c>
-      <c r="H18" s="78">
+      <c r="H18" s="77">
         <v>0.38640000000000002</v>
       </c>
       <c r="K18" s="49"/>
@@ -10884,8 +10879,8 @@
         <f t="shared" si="0"/>
         <v>0.12280783272485894</v>
       </c>
-      <c r="U18" s="84"/>
-      <c r="V18" s="81"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="87"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="56">
@@ -10905,14 +10900,14 @@
         <v>ct</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="75">
+      <c r="F19" s="74">
         <v>2042.57</v>
       </c>
-      <c r="G19" s="74">
+      <c r="G19" s="73">
         <f t="shared" si="2"/>
         <v>1.1423619707848446E-2</v>
       </c>
-      <c r="H19" s="78">
+      <c r="H19" s="77">
         <v>0.91</v>
       </c>
       <c r="K19" s="49"/>
@@ -10923,8 +10918,8 @@
         <f t="shared" si="0"/>
         <v>0.18575885120079233</v>
       </c>
-      <c r="U19" s="84"/>
-      <c r="V19" s="81"/>
+      <c r="U19" s="90"/>
+      <c r="V19" s="87"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="56">
@@ -10944,14 +10939,14 @@
         <v>ct</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="75">
+      <c r="F20" s="74">
         <v>1505.96</v>
       </c>
-      <c r="G20" s="74">
+      <c r="G20" s="73">
         <f t="shared" si="2"/>
         <v>6.6360818350898923E-2</v>
       </c>
-      <c r="H20" s="78">
+      <c r="H20" s="77">
         <v>0.87139999999999995</v>
       </c>
       <c r="K20" s="49"/>
@@ -10962,8 +10957,8 @@
         <f t="shared" si="0"/>
         <v>0.17690638561686292</v>
       </c>
-      <c r="U20" s="86"/>
-      <c r="V20" s="87"/>
+      <c r="U20" s="92"/>
+      <c r="V20" s="93"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="56">
@@ -10983,8 +10978,8 @@
         <v>mr</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="79"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="78"/>
       <c r="J21" s="31">
         <v>1681.62</v>
       </c>
@@ -11002,10 +10997,10 @@
         <f t="shared" si="0"/>
         <v>5.9219518043400046E-2</v>
       </c>
-      <c r="U21" s="83" t="s">
+      <c r="U21" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="V21" s="80" t="s">
+      <c r="V21" s="86" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11027,8 +11022,8 @@
         <v>mr</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="79"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="78"/>
       <c r="J22" s="31">
         <v>1934.24</v>
       </c>
@@ -11046,8 +11041,8 @@
         <f t="shared" si="0"/>
         <v>0.57086158977209567</v>
       </c>
-      <c r="U22" s="84"/>
-      <c r="V22" s="81"/>
+      <c r="U22" s="90"/>
+      <c r="V22" s="87"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="56">
@@ -11067,8 +11062,8 @@
         <v>mr</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="79"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="78"/>
       <c r="J23" s="31">
         <v>1276.94</v>
       </c>
@@ -11086,8 +11081,8 @@
         <f t="shared" si="0"/>
         <v>1.0577267837934744E-2</v>
       </c>
-      <c r="U23" s="84"/>
-      <c r="V23" s="81"/>
+      <c r="U23" s="90"/>
+      <c r="V23" s="87"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="56">
@@ -11107,8 +11102,8 @@
         <v>mr</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="79"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="78"/>
       <c r="J24" s="31">
         <v>1012.37</v>
       </c>
@@ -11123,8 +11118,8 @@
         <f t="shared" si="0"/>
         <v>0.16852443154329944</v>
       </c>
-      <c r="U24" s="84"/>
-      <c r="V24" s="81"/>
+      <c r="U24" s="90"/>
+      <c r="V24" s="87"/>
     </row>
     <row r="25" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="56">
@@ -11144,14 +11139,14 @@
         <v>ct</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="75">
+      <c r="F25" s="74">
         <v>1775.63</v>
       </c>
-      <c r="G25" s="74">
+      <c r="G25" s="73">
         <f t="shared" si="2"/>
         <v>8.5292602513908883E-2</v>
       </c>
-      <c r="H25" s="78">
+      <c r="H25" s="77">
         <v>0.89490000000000003</v>
       </c>
       <c r="K25" s="49"/>
@@ -11162,8 +11157,8 @@
         <f t="shared" si="0"/>
         <v>0.24993303111477427</v>
       </c>
-      <c r="U25" s="85"/>
-      <c r="V25" s="82"/>
+      <c r="U25" s="91"/>
+      <c r="V25" s="88"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="56">
@@ -11183,8 +11178,8 @@
         <v>mr</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="79"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="78"/>
       <c r="J26" s="31">
         <v>1244.6600000000001</v>
       </c>
@@ -11202,10 +11197,10 @@
         <f t="shared" si="0"/>
         <v>0.17338942939784374</v>
       </c>
-      <c r="U26" s="101" t="s">
+      <c r="U26" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="V26" s="102"/>
+      <c r="V26" s="101"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="56">
@@ -11225,8 +11220,8 @@
         <v>mr</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="79"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="78"/>
       <c r="J27" s="31">
         <v>1524.13</v>
       </c>
@@ -11244,8 +11239,8 @@
         <f t="shared" si="0"/>
         <v>0.13298224292755387</v>
       </c>
-      <c r="U27" s="103"/>
-      <c r="V27" s="104"/>
+      <c r="U27" s="102"/>
+      <c r="V27" s="103"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="56">
@@ -11265,14 +11260,14 @@
         <v>ct</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="75">
+      <c r="F28" s="74">
         <v>1171.33</v>
       </c>
-      <c r="G28" s="74">
+      <c r="G28" s="73">
         <f t="shared" si="2"/>
         <v>1.2785503581963821E-2</v>
       </c>
-      <c r="H28" s="78">
+      <c r="H28" s="77">
         <v>0.95209999999999995</v>
       </c>
       <c r="K28" s="49"/>
@@ -11283,8 +11278,8 @@
         <f t="shared" si="0"/>
         <v>3.0172777075431905E-2</v>
       </c>
-      <c r="U28" s="103"/>
-      <c r="V28" s="104"/>
+      <c r="U28" s="102"/>
+      <c r="V28" s="103"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="56">
@@ -11304,8 +11299,8 @@
         <v>mr</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="79"/>
+      <c r="G29" s="73"/>
+      <c r="H29" s="78"/>
       <c r="J29" s="31">
         <v>2006.6</v>
       </c>
@@ -11320,8 +11315,8 @@
         <f t="shared" si="0"/>
         <v>4.6656784371856573E-2</v>
       </c>
-      <c r="U29" s="103"/>
-      <c r="V29" s="104"/>
+      <c r="U29" s="102"/>
+      <c r="V29" s="103"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="56">
@@ -11341,14 +11336,14 @@
         <v>ct</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="75">
+      <c r="F30" s="74">
         <v>1328.99</v>
       </c>
-      <c r="G30" s="74">
+      <c r="G30" s="73">
         <f t="shared" si="2"/>
         <v>8.8742124041600659E-3</v>
       </c>
-      <c r="H30" s="78">
+      <c r="H30" s="77">
         <v>0.93149999999999999</v>
       </c>
       <c r="K30" s="49"/>
@@ -11359,8 +11354,8 @@
         <f t="shared" si="0"/>
         <v>0.11378577393152652</v>
       </c>
-      <c r="U30" s="103"/>
-      <c r="V30" s="104"/>
+      <c r="U30" s="102"/>
+      <c r="V30" s="103"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="56">
@@ -11380,8 +11375,8 @@
         <v>mr</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="79"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="78"/>
       <c r="J31" s="31">
         <v>2030.28</v>
       </c>
@@ -11399,8 +11394,8 @@
         <f t="shared" si="0"/>
         <v>0.32840989044125041</v>
       </c>
-      <c r="U31" s="103"/>
-      <c r="V31" s="104"/>
+      <c r="U31" s="102"/>
+      <c r="V31" s="103"/>
     </row>
     <row r="32" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="56">
@@ -11420,14 +11415,14 @@
         <v>ct</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="75">
+      <c r="F32" s="74">
         <v>1607.99</v>
       </c>
-      <c r="G32" s="74">
+      <c r="G32" s="73">
         <f t="shared" si="2"/>
         <v>6.3978032157745029E-2</v>
       </c>
-      <c r="H32" s="78">
+      <c r="H32" s="77">
         <v>0.91510000000000002</v>
       </c>
       <c r="K32" s="49"/>
@@ -11438,8 +11433,8 @@
         <f t="shared" si="0"/>
         <v>0.12921987692714879</v>
       </c>
-      <c r="U32" s="105"/>
-      <c r="V32" s="106"/>
+      <c r="U32" s="104"/>
+      <c r="V32" s="105"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="56">
@@ -11459,14 +11454,14 @@
         <v>ct</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="75">
+      <c r="F33" s="74">
         <v>1054.97</v>
       </c>
-      <c r="G33" s="74">
+      <c r="G33" s="73">
         <f t="shared" si="2"/>
         <v>0.12486934881791785</v>
       </c>
-      <c r="H33" s="78">
+      <c r="H33" s="77">
         <v>0.8347</v>
       </c>
       <c r="K33" s="49"/>
@@ -11496,14 +11491,14 @@
         <v>ct</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="75">
+      <c r="F34" s="74">
         <v>1566.83</v>
       </c>
-      <c r="G34" s="74">
+      <c r="G34" s="73">
         <f t="shared" si="2"/>
         <v>6.5073553028842301E-3</v>
       </c>
-      <c r="H34" s="78">
+      <c r="H34" s="77">
         <v>0.95640000000000003</v>
       </c>
       <c r="K34" s="49"/>
@@ -11533,8 +11528,8 @@
         <v>mr</v>
       </c>
       <c r="E35" s="3"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="79"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="78"/>
       <c r="J35" s="31">
         <v>1336.71</v>
       </c>
@@ -11574,14 +11569,14 @@
         <v>ct</v>
       </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="75">
+      <c r="F36" s="74">
         <v>1150.19</v>
       </c>
-      <c r="G36" s="74">
+      <c r="G36" s="73">
         <f t="shared" si="2"/>
         <v>3.7048056983139614E-2</v>
       </c>
-      <c r="H36" s="78">
+      <c r="H36" s="77">
         <v>0.89890000000000003</v>
       </c>
       <c r="K36" s="49"/>
@@ -11614,8 +11609,8 @@
         <v>mr</v>
       </c>
       <c r="E37" s="3"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="79"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="78"/>
       <c r="J37" s="31">
         <v>1109.0999999999999</v>
       </c>
@@ -11652,8 +11647,8 @@
         <v>mr</v>
       </c>
       <c r="E38" s="3"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="79"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="78"/>
       <c r="J38" s="31">
         <v>1684.75</v>
       </c>
@@ -11690,14 +11685,14 @@
         <v>ct</v>
       </c>
       <c r="E39" s="3"/>
-      <c r="F39" s="75">
+      <c r="F39" s="74">
         <v>3079.66</v>
       </c>
-      <c r="G39" s="74">
+      <c r="G39" s="73">
         <f t="shared" si="2"/>
         <v>0.11750007163939594</v>
       </c>
-      <c r="H39" s="78">
+      <c r="H39" s="77">
         <v>0.92549999999999999</v>
       </c>
       <c r="K39" s="49"/>
@@ -11726,8 +11721,8 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>0</v>
       </c>
-      <c r="G40" s="74"/>
-      <c r="H40" s="79"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="78"/>
       <c r="K40" s="49"/>
       <c r="P40" s="21" t="s">
         <v>34</v>
@@ -11751,8 +11746,8 @@
         <v>mr</v>
       </c>
       <c r="E41" s="3"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="79"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="78"/>
       <c r="J41" s="31">
         <v>1217.24</v>
       </c>
@@ -11789,8 +11784,8 @@
         <v>mr</v>
       </c>
       <c r="E42" s="3"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="79"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="78"/>
       <c r="J42" s="31">
         <v>2674.48</v>
       </c>
@@ -11827,8 +11822,8 @@
         <v>mr</v>
       </c>
       <c r="E43" s="3"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="79"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="78"/>
       <c r="J43" s="64">
         <v>2161.6999999999998</v>
       </c>
@@ -11865,14 +11860,14 @@
         <v>ct</v>
       </c>
       <c r="E44" s="3"/>
-      <c r="F44" s="75">
+      <c r="F44" s="74">
         <v>2911.33</v>
       </c>
-      <c r="G44" s="74">
+      <c r="G44" s="73">
         <f t="shared" si="2"/>
         <v>0.20211302345976764</v>
       </c>
-      <c r="H44" s="79">
+      <c r="H44" s="78">
         <v>0.85880000000000001</v>
       </c>
       <c r="K44" s="49"/>
@@ -11905,8 +11900,8 @@
         <v>mr</v>
       </c>
       <c r="E45" s="3"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="79"/>
+      <c r="G45" s="73"/>
+      <c r="H45" s="78"/>
       <c r="K45" s="49"/>
       <c r="N45" s="60">
         <v>2483.09</v>
@@ -11937,14 +11932,14 @@
         <v>ct</v>
       </c>
       <c r="E46" s="3"/>
-      <c r="F46" s="75">
+      <c r="F46" s="74">
         <v>1306.32</v>
       </c>
-      <c r="G46" s="74">
+      <c r="G46" s="73">
         <f t="shared" si="2"/>
         <v>5.4029092588316644E-3</v>
       </c>
-      <c r="H46" s="78">
+      <c r="H46" s="77">
         <v>0.91159999999999997</v>
       </c>
       <c r="K46" s="49"/>
@@ -11974,8 +11969,8 @@
         <v>mr</v>
       </c>
       <c r="E47" s="3"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="79"/>
+      <c r="G47" s="73"/>
+      <c r="H47" s="78"/>
       <c r="J47" s="31">
         <v>1224.79</v>
       </c>
@@ -12012,14 +12007,14 @@
         <v>ct</v>
       </c>
       <c r="E48" s="3"/>
-      <c r="F48" s="75">
+      <c r="F48" s="74">
         <v>1284.98</v>
       </c>
-      <c r="G48" s="74">
+      <c r="G48" s="73">
         <f t="shared" si="2"/>
         <v>1.0335797905114042E-2</v>
       </c>
-      <c r="H48" s="78">
+      <c r="H48" s="77">
         <v>0.91169999999999995</v>
       </c>
       <c r="K48" s="49"/>
@@ -12049,14 +12044,14 @@
         <v>ct</v>
       </c>
       <c r="E49" s="3"/>
-      <c r="F49" s="75">
+      <c r="F49" s="74">
         <v>1320.03</v>
       </c>
-      <c r="G49" s="74">
+      <c r="G49" s="73">
         <f t="shared" si="2"/>
         <v>3.0174123870398896E-2</v>
       </c>
-      <c r="H49" s="78">
+      <c r="H49" s="77">
         <v>0.95179999999999998</v>
       </c>
       <c r="K49" s="49"/>
@@ -12086,8 +12081,8 @@
         <v>mr</v>
       </c>
       <c r="E50" s="3"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="79"/>
+      <c r="G50" s="73"/>
+      <c r="H50" s="78"/>
       <c r="J50" s="31">
         <v>1208.56</v>
       </c>
@@ -12124,8 +12119,8 @@
         <v>mr</v>
       </c>
       <c r="E51" s="3"/>
-      <c r="G51" s="74"/>
-      <c r="H51" s="79"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="78"/>
       <c r="J51" s="31">
         <v>1437.44</v>
       </c>
@@ -12162,14 +12157,14 @@
         <v>ct</v>
       </c>
       <c r="E52" s="3"/>
-      <c r="F52" s="75">
+      <c r="F52" s="74">
         <v>204.72800000000001</v>
       </c>
-      <c r="G52" s="74">
+      <c r="G52" s="73">
         <f t="shared" si="2"/>
         <v>0.86539907955292561</v>
       </c>
-      <c r="H52" s="79">
+      <c r="H52" s="78">
         <v>0.2366</v>
       </c>
       <c r="K52" s="49"/>
@@ -12199,14 +12194,14 @@
         <v>ct</v>
       </c>
       <c r="E53" s="3"/>
-      <c r="F53" s="75">
+      <c r="F53" s="74">
         <v>2132.17</v>
       </c>
-      <c r="G53" s="74">
+      <c r="G53" s="73">
         <f t="shared" si="2"/>
         <v>0.56650503269414465</v>
       </c>
-      <c r="H53" s="79">
+      <c r="H53" s="78">
         <v>0.91200000000000003</v>
       </c>
       <c r="K53" s="49"/>
@@ -12236,14 +12231,14 @@
         <v>ct</v>
       </c>
       <c r="E54" s="3"/>
-      <c r="F54" s="75">
+      <c r="F54" s="74">
         <v>3118.28</v>
       </c>
-      <c r="G54" s="74">
+      <c r="G54" s="73">
         <f t="shared" si="2"/>
         <v>3.1893841622820114E-2</v>
       </c>
-      <c r="H54" s="78">
+      <c r="H54" s="77">
         <v>0.90269999999999995</v>
       </c>
       <c r="K54" s="49"/>
@@ -12273,14 +12268,14 @@
         <v>ct</v>
       </c>
       <c r="E55" s="3"/>
-      <c r="F55" s="75">
+      <c r="F55" s="74">
         <v>1897.91</v>
       </c>
-      <c r="G55" s="74">
+      <c r="G55" s="73">
         <f t="shared" si="2"/>
         <v>0.14055608386541688</v>
       </c>
-      <c r="H55" s="78">
+      <c r="H55" s="77">
         <v>0.90700000000000003</v>
       </c>
       <c r="K55" s="49"/>
@@ -12310,8 +12305,8 @@
         <v>mr</v>
       </c>
       <c r="E56" s="3"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="79"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="78"/>
       <c r="J56" s="31">
         <v>1988.71</v>
       </c>
@@ -12348,8 +12343,8 @@
         <v>mr</v>
       </c>
       <c r="E57" s="3"/>
-      <c r="G57" s="74"/>
-      <c r="H57" s="79"/>
+      <c r="G57" s="73"/>
+      <c r="H57" s="78"/>
       <c r="J57" s="31">
         <v>2184.8000000000002</v>
       </c>
@@ -12386,14 +12381,14 @@
         <v>ct</v>
       </c>
       <c r="E58" s="3"/>
-      <c r="F58" s="75">
+      <c r="F58" s="74">
         <v>1604.75</v>
       </c>
-      <c r="G58" s="74">
+      <c r="G58" s="73">
         <f t="shared" si="2"/>
         <v>2.4221342864437098E-2</v>
       </c>
-      <c r="H58" s="78">
+      <c r="H58" s="77">
         <v>0.90449999999999997</v>
       </c>
       <c r="K58" s="49"/>
@@ -12423,14 +12418,14 @@
         <v>ct</v>
       </c>
       <c r="E59" s="3"/>
-      <c r="F59" s="75">
+      <c r="F59" s="74">
         <v>1791.65</v>
       </c>
-      <c r="G59" s="74">
+      <c r="G59" s="73">
         <f t="shared" si="2"/>
         <v>2.461969575660539E-2</v>
       </c>
-      <c r="H59" s="78">
+      <c r="H59" s="77">
         <v>0.92800000000000005</v>
       </c>
       <c r="K59" s="49"/>
@@ -12460,14 +12455,14 @@
         <v>ct</v>
       </c>
       <c r="E60" s="3"/>
-      <c r="F60" s="75">
+      <c r="F60" s="74">
         <v>1426.29</v>
       </c>
-      <c r="G60" s="74">
+      <c r="G60" s="73">
         <f t="shared" si="2"/>
         <v>5.1858007046466793E-2</v>
       </c>
-      <c r="H60" s="78">
+      <c r="H60" s="77">
         <v>0.93379999999999996</v>
       </c>
       <c r="K60" s="49"/>
@@ -12497,14 +12492,14 @@
         <v>ct</v>
       </c>
       <c r="E61" s="3"/>
-      <c r="F61" s="75">
+      <c r="F61" s="74">
         <v>1965.81</v>
       </c>
-      <c r="G61" s="74">
+      <c r="G61" s="73">
         <f t="shared" si="2"/>
         <v>0.70670496083550927</v>
       </c>
-      <c r="H61" s="78">
+      <c r="H61" s="77">
         <v>0.44429999999999997</v>
       </c>
       <c r="K61" s="49"/>
@@ -12534,14 +12529,14 @@
         <v>ct</v>
       </c>
       <c r="E62" s="3"/>
-      <c r="F62" s="75">
+      <c r="F62" s="74">
         <v>1285.73</v>
       </c>
-      <c r="G62" s="74">
+      <c r="G62" s="73">
         <f t="shared" si="2"/>
         <v>0.17427910859931919</v>
       </c>
-      <c r="H62" s="78">
+      <c r="H62" s="77">
         <v>0.85040000000000004</v>
       </c>
       <c r="K62" s="49"/>
@@ -12571,8 +12566,8 @@
         <v>mr</v>
       </c>
       <c r="E63" s="3"/>
-      <c r="G63" s="74"/>
-      <c r="H63" s="79"/>
+      <c r="G63" s="73"/>
+      <c r="H63" s="78"/>
       <c r="J63" s="31">
         <v>1588.84</v>
       </c>
@@ -12609,14 +12604,14 @@
         <v>ct</v>
       </c>
       <c r="E64" s="3"/>
-      <c r="F64" s="75">
+      <c r="F64" s="74">
         <v>1369.12</v>
       </c>
-      <c r="G64" s="74">
+      <c r="G64" s="73">
         <f t="shared" si="2"/>
         <v>0.16511982437953546</v>
       </c>
-      <c r="H64" s="78">
+      <c r="H64" s="77">
         <v>0.83089999999999997</v>
       </c>
       <c r="K64" s="49"/>
@@ -12646,14 +12641,14 @@
         <v>ct</v>
       </c>
       <c r="E65" s="3"/>
-      <c r="F65" s="75">
+      <c r="F65" s="74">
         <v>1197.28</v>
       </c>
-      <c r="G65" s="74">
+      <c r="G65" s="73">
         <f t="shared" si="2"/>
         <v>0.50400596545010157</v>
       </c>
-      <c r="H65" s="78">
+      <c r="H65" s="77">
         <v>0.65049999999999997</v>
       </c>
       <c r="K65" s="49"/>
@@ -12683,14 +12678,14 @@
         <v>ct</v>
       </c>
       <c r="E66" s="3"/>
-      <c r="F66" s="75">
+      <c r="F66" s="74">
         <v>1388.7</v>
       </c>
-      <c r="G66" s="74">
+      <c r="G66" s="73">
         <f t="shared" si="2"/>
         <v>8.6621941594317312E-2</v>
       </c>
-      <c r="H66" s="78">
+      <c r="H66" s="77">
         <v>0.93240000000000001</v>
       </c>
       <c r="K66" s="49"/>
@@ -12723,8 +12718,8 @@
         <v>mr</v>
       </c>
       <c r="E67" s="3"/>
-      <c r="G67" s="74"/>
-      <c r="H67" s="79"/>
+      <c r="G67" s="73"/>
+      <c r="H67" s="78"/>
       <c r="J67" s="31">
         <v>2389.33</v>
       </c>
@@ -12758,8 +12753,8 @@
         <v>mr</v>
       </c>
       <c r="E68" s="3"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="79"/>
+      <c r="G68" s="73"/>
+      <c r="H68" s="78"/>
       <c r="J68" s="31">
         <v>1361.91</v>
       </c>
@@ -12796,14 +12791,14 @@
         <v>ct</v>
       </c>
       <c r="E69" s="3"/>
-      <c r="F69" s="75">
+      <c r="F69" s="74">
         <v>2330.11</v>
       </c>
-      <c r="G69" s="74">
+      <c r="G69" s="73">
         <f t="shared" si="2"/>
         <v>4.8235438281186052E-2</v>
       </c>
-      <c r="H69" s="78">
+      <c r="H69" s="77">
         <v>0.94479999999999997</v>
       </c>
       <c r="K69" s="49"/>
@@ -12833,8 +12828,8 @@
         <v>mr</v>
       </c>
       <c r="E70" s="3"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="79"/>
+      <c r="G70" s="73"/>
+      <c r="H70" s="78"/>
       <c r="J70" s="31">
         <v>1873.03</v>
       </c>
@@ -12871,8 +12866,8 @@
         <v>mr</v>
       </c>
       <c r="E71" s="3"/>
-      <c r="G71" s="74"/>
-      <c r="H71" s="79"/>
+      <c r="G71" s="73"/>
+      <c r="H71" s="78"/>
       <c r="J71" s="31">
         <v>2739.91</v>
       </c>
@@ -12909,8 +12904,8 @@
         <v>mr</v>
       </c>
       <c r="E72" s="3"/>
-      <c r="G72" s="74"/>
-      <c r="H72" s="79"/>
+      <c r="G72" s="73"/>
+      <c r="H72" s="78"/>
       <c r="J72" s="64">
         <v>2166.4899999999998</v>
       </c>
@@ -12947,14 +12942,14 @@
         <v>ct</v>
       </c>
       <c r="E73" s="3"/>
-      <c r="F73" s="75">
+      <c r="F73" s="74">
         <v>1878.56</v>
       </c>
-      <c r="G73" s="74">
+      <c r="G73" s="73">
         <f t="shared" ref="G73:G102" si="7">+ABS((C73-F73)/C73)</f>
         <v>3.3662551440329244E-2</v>
       </c>
-      <c r="H73" s="78">
+      <c r="H73" s="77">
         <v>0.9204</v>
       </c>
       <c r="K73" s="49"/>
@@ -12987,14 +12982,14 @@
         <v>ct</v>
       </c>
       <c r="E74" s="3"/>
-      <c r="F74" s="75">
+      <c r="F74" s="74">
         <v>1489.32</v>
       </c>
-      <c r="G74" s="74">
+      <c r="G74" s="73">
         <f t="shared" si="7"/>
         <v>2.8302994715208526E-2</v>
       </c>
-      <c r="H74" s="78">
+      <c r="H74" s="77">
         <v>0.95569999999999999</v>
       </c>
       <c r="K74" s="49"/>
@@ -13024,8 +13019,8 @@
         <v>mr</v>
       </c>
       <c r="E75" s="3"/>
-      <c r="G75" s="74"/>
-      <c r="H75" s="79"/>
+      <c r="G75" s="73"/>
+      <c r="H75" s="78"/>
       <c r="J75" s="31">
         <v>1026.5999999999999</v>
       </c>
@@ -13062,8 +13057,8 @@
         <v>mr</v>
       </c>
       <c r="E76" s="3"/>
-      <c r="G76" s="74"/>
-      <c r="H76" s="79"/>
+      <c r="G76" s="73"/>
+      <c r="H76" s="78"/>
       <c r="J76" s="31">
         <v>1467.93</v>
       </c>
@@ -13100,14 +13095,14 @@
         <v>ct</v>
       </c>
       <c r="E77" s="3"/>
-      <c r="F77" s="75">
+      <c r="F77" s="74">
         <v>1673.78</v>
       </c>
-      <c r="G77" s="74">
+      <c r="G77" s="73">
         <f t="shared" si="7"/>
         <v>5.0643399661038271E-2</v>
       </c>
-      <c r="H77" s="78">
+      <c r="H77" s="77">
         <v>0.9022</v>
       </c>
       <c r="K77" s="49"/>
@@ -13137,14 +13132,14 @@
         <v>ct</v>
       </c>
       <c r="E78" s="3"/>
-      <c r="F78" s="75">
+      <c r="F78" s="74">
         <v>1796.36</v>
       </c>
-      <c r="G78" s="74">
+      <c r="G78" s="73">
         <f t="shared" si="7"/>
         <v>0.1339086832843161</v>
       </c>
-      <c r="H78" s="78">
+      <c r="H78" s="77">
         <v>0.90280000000000005</v>
       </c>
       <c r="K78" s="49"/>
@@ -13174,8 +13169,8 @@
         <v>mr</v>
       </c>
       <c r="E79" s="3"/>
-      <c r="G79" s="74"/>
-      <c r="H79" s="79"/>
+      <c r="G79" s="73"/>
+      <c r="H79" s="78"/>
       <c r="J79" s="31">
         <v>1922.03</v>
       </c>
@@ -13212,8 +13207,8 @@
         <v>mr</v>
       </c>
       <c r="E80" s="3"/>
-      <c r="G80" s="74"/>
-      <c r="H80" s="79"/>
+      <c r="G80" s="73"/>
+      <c r="H80" s="78"/>
       <c r="J80" s="31">
         <v>2259.59</v>
       </c>
@@ -13250,8 +13245,8 @@
         <v>mr</v>
       </c>
       <c r="E81" s="3"/>
-      <c r="G81" s="74"/>
-      <c r="H81" s="79"/>
+      <c r="G81" s="73"/>
+      <c r="H81" s="78"/>
       <c r="J81" s="31">
         <v>1426.86</v>
       </c>
@@ -13288,8 +13283,8 @@
         <v>mr</v>
       </c>
       <c r="E82" s="3"/>
-      <c r="G82" s="74"/>
-      <c r="H82" s="79"/>
+      <c r="G82" s="73"/>
+      <c r="H82" s="78"/>
       <c r="J82" s="31">
         <v>1440.9</v>
       </c>
@@ -13326,8 +13321,8 @@
         <v>mr</v>
       </c>
       <c r="E83" s="3"/>
-      <c r="G83" s="74"/>
-      <c r="H83" s="79"/>
+      <c r="G83" s="73"/>
+      <c r="H83" s="78"/>
       <c r="J83" s="31">
         <v>1418.24</v>
       </c>
@@ -13364,8 +13359,8 @@
         <v>mr</v>
       </c>
       <c r="E84" s="3"/>
-      <c r="G84" s="74"/>
-      <c r="H84" s="79"/>
+      <c r="G84" s="73"/>
+      <c r="H84" s="78"/>
       <c r="J84" s="31">
         <v>2080.9699999999998</v>
       </c>
@@ -13402,14 +13397,14 @@
         <v>ct</v>
       </c>
       <c r="E85" s="3"/>
-      <c r="F85" s="75">
+      <c r="F85" s="74">
         <v>1902.79</v>
       </c>
-      <c r="G85" s="74">
+      <c r="G85" s="73">
         <f t="shared" si="7"/>
         <v>7.7882238914465732E-2</v>
       </c>
-      <c r="H85" s="78">
+      <c r="H85" s="77">
         <v>0.87360000000000004</v>
       </c>
       <c r="K85" s="49"/>
@@ -13438,8 +13433,8 @@
         <v>0</v>
       </c>
       <c r="E86" s="3"/>
-      <c r="G86" s="74"/>
-      <c r="H86" s="79"/>
+      <c r="G86" s="73"/>
+      <c r="H86" s="78"/>
       <c r="K86" s="49"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -13460,8 +13455,8 @@
         <v>mr</v>
       </c>
       <c r="E87" s="3"/>
-      <c r="G87" s="74"/>
-      <c r="H87" s="79"/>
+      <c r="G87" s="73"/>
+      <c r="H87" s="78"/>
       <c r="J87" s="31">
         <v>2386.02</v>
       </c>
@@ -13498,14 +13493,14 @@
         <v>ct</v>
       </c>
       <c r="E88" s="3"/>
-      <c r="F88" s="75">
+      <c r="F88" s="74">
         <v>864.98</v>
       </c>
-      <c r="G88" s="74">
+      <c r="G88" s="73">
         <f t="shared" si="7"/>
         <v>1.5234741784037579E-2</v>
       </c>
-      <c r="H88" s="78">
+      <c r="H88" s="77">
         <v>0.9012</v>
       </c>
       <c r="K88" s="49"/>
@@ -13535,8 +13530,8 @@
         <v>mr</v>
       </c>
       <c r="E89" s="3"/>
-      <c r="G89" s="74"/>
-      <c r="H89" s="79"/>
+      <c r="G89" s="73"/>
+      <c r="H89" s="78"/>
       <c r="J89" s="31">
         <v>2811.37</v>
       </c>
@@ -13573,14 +13568,14 @@
         <v>ct</v>
       </c>
       <c r="E90" s="3"/>
-      <c r="F90" s="75">
+      <c r="F90" s="74">
         <v>1043.18</v>
       </c>
-      <c r="G90" s="74">
+      <c r="G90" s="73">
         <f t="shared" si="7"/>
         <v>0.62546942878684519</v>
       </c>
-      <c r="H90" s="78">
+      <c r="H90" s="77">
         <v>0.8448</v>
       </c>
       <c r="K90" s="49"/>
@@ -13613,8 +13608,8 @@
         <v>mr</v>
       </c>
       <c r="E91" s="3"/>
-      <c r="G91" s="74"/>
-      <c r="H91" s="79"/>
+      <c r="G91" s="73"/>
+      <c r="H91" s="78"/>
       <c r="J91" s="31">
         <v>3751.2</v>
       </c>
@@ -13651,8 +13646,8 @@
         <v>mr</v>
       </c>
       <c r="E92" s="3"/>
-      <c r="G92" s="74"/>
-      <c r="H92" s="79"/>
+      <c r="G92" s="73"/>
+      <c r="H92" s="78"/>
       <c r="J92" s="31">
         <v>2320.0300000000002</v>
       </c>
@@ -13689,8 +13684,8 @@
         <v>mr</v>
       </c>
       <c r="E93" s="3"/>
-      <c r="G93" s="74"/>
-      <c r="H93" s="79"/>
+      <c r="G93" s="73"/>
+      <c r="H93" s="78"/>
       <c r="J93" s="31">
         <v>1816.86</v>
       </c>
@@ -13727,8 +13722,8 @@
         <v>mr</v>
       </c>
       <c r="E94" s="3"/>
-      <c r="G94" s="74"/>
-      <c r="H94" s="79"/>
+      <c r="G94" s="73"/>
+      <c r="H94" s="78"/>
       <c r="J94" s="31">
         <v>1399.21</v>
       </c>
@@ -13765,8 +13760,8 @@
         <v>mr</v>
       </c>
       <c r="E95" s="3"/>
-      <c r="G95" s="74"/>
-      <c r="H95" s="79"/>
+      <c r="G95" s="73"/>
+      <c r="H95" s="78"/>
       <c r="J95" s="31">
         <v>2253.86</v>
       </c>
@@ -13803,8 +13798,8 @@
         <v>mr</v>
       </c>
       <c r="E96" s="3"/>
-      <c r="G96" s="74"/>
-      <c r="H96" s="79"/>
+      <c r="G96" s="73"/>
+      <c r="H96" s="78"/>
       <c r="J96" s="31">
         <v>2649.56</v>
       </c>
@@ -13841,8 +13836,8 @@
         <v>mr</v>
       </c>
       <c r="E97" s="3"/>
-      <c r="G97" s="74"/>
-      <c r="H97" s="79"/>
+      <c r="G97" s="73"/>
+      <c r="H97" s="78"/>
       <c r="J97" s="31">
         <v>2032.49</v>
       </c>
@@ -13879,8 +13874,8 @@
         <v>mr</v>
       </c>
       <c r="E98" s="3"/>
-      <c r="G98" s="74"/>
-      <c r="H98" s="79"/>
+      <c r="G98" s="73"/>
+      <c r="H98" s="78"/>
       <c r="J98" s="31">
         <v>1989.88</v>
       </c>
@@ -13917,8 +13912,8 @@
         <v>mr</v>
       </c>
       <c r="E99" s="3"/>
-      <c r="G99" s="74"/>
-      <c r="H99" s="79"/>
+      <c r="G99" s="73"/>
+      <c r="H99" s="78"/>
       <c r="J99" s="31">
         <v>1235.1300000000001</v>
       </c>
@@ -13955,8 +13950,8 @@
         <v>mr</v>
       </c>
       <c r="E100" s="3"/>
-      <c r="G100" s="74"/>
-      <c r="H100" s="79"/>
+      <c r="G100" s="73"/>
+      <c r="H100" s="78"/>
       <c r="J100" s="31">
         <v>2386.73</v>
       </c>
@@ -13993,8 +13988,8 @@
         <v>mr</v>
       </c>
       <c r="E101" s="3"/>
-      <c r="G101" s="74"/>
-      <c r="H101" s="79"/>
+      <c r="G101" s="73"/>
+      <c r="H101" s="78"/>
       <c r="J101" s="31">
         <v>1489.94</v>
       </c>
@@ -14031,14 +14026,14 @@
         <v>ct</v>
       </c>
       <c r="E102" s="3"/>
-      <c r="F102" s="75">
+      <c r="F102" s="74">
         <v>3521.54</v>
       </c>
-      <c r="G102" s="74">
+      <c r="G102" s="73">
         <f t="shared" si="7"/>
         <v>4.3007772161530573E-2</v>
       </c>
-      <c r="H102" s="78">
+      <c r="H102" s="77">
         <v>0.93300000000000005</v>
       </c>
       <c r="K102" s="49"/>
@@ -14071,7 +14066,7 @@
         <v>mr</v>
       </c>
       <c r="E103" s="3"/>
-      <c r="G103" s="74"/>
+      <c r="G103" s="73"/>
       <c r="J103" s="64">
         <v>1988.8</v>
       </c>
@@ -14111,7 +14106,7 @@
         <v>mr</v>
       </c>
       <c r="E104" s="3"/>
-      <c r="G104" s="74"/>
+      <c r="G104" s="73"/>
       <c r="J104" s="31">
         <v>1781.79</v>
       </c>
@@ -14137,10 +14132,10 @@
       <c r="K106" s="50"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B107" s="88" t="s">
+      <c r="B107" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="C107" s="89"/>
+      <c r="C107" s="80"/>
       <c r="D107" s="47">
         <f>COUNTIF(D2:D104,"=mr")</f>
         <v>55</v>
@@ -14148,10 +14143,10 @@
       <c r="K107" s="50"/>
     </row>
     <row r="108" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="90" t="s">
+      <c r="B108" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="C108" s="91"/>
+      <c r="C108" s="82"/>
       <c r="D108" s="48">
         <f>COUNTIF(D2:D104,"=ct")</f>
         <v>46</v>
@@ -14509,17 +14504,17 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="106" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="109"/>
-      <c r="F2" s="107" t="s">
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
+      <c r="F2" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="109"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="108"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="31">
@@ -16478,1720 +16473,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BFEF96-1493-46B5-BD73-B520A6D93575}">
-  <dimension ref="A1:E103"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="68">
-        <v>0.86875000000000002</v>
-      </c>
-      <c r="E1">
-        <v>1574.15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="68">
-        <v>0.87013888888888891</v>
-      </c>
-      <c r="E2">
-        <v>2308.64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="68">
-        <v>0.87152777777777779</v>
-      </c>
-      <c r="E3">
-        <v>1385.37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="68">
-        <v>0.87222222222222223</v>
-      </c>
-      <c r="E4">
-        <v>1831.56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="68">
-        <v>0.87361111111111101</v>
-      </c>
-      <c r="E5">
-        <v>2310.2399999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="68">
-        <v>0.87430555555555556</v>
-      </c>
-      <c r="E6">
-        <v>1426.42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="68">
-        <v>0.87569444444444444</v>
-      </c>
-      <c r="E7">
-        <v>880.64200000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="68">
-        <v>0.87708333333333333</v>
-      </c>
-      <c r="E8">
-        <v>1430.88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="68">
-        <v>0.87777777777777777</v>
-      </c>
-      <c r="E9">
-        <v>1519.63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="68">
-        <v>0.87916666666666676</v>
-      </c>
-      <c r="E10">
-        <v>1364.79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="68">
-        <v>0.88055555555555554</v>
-      </c>
-      <c r="E11">
-        <v>1398.73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="68">
-        <v>0.88124999999999998</v>
-      </c>
-      <c r="E12">
-        <v>1702.24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="68">
-        <v>0.88263888888888886</v>
-      </c>
-      <c r="E13">
-        <v>1526.97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="68">
-        <v>0.88402777777777775</v>
-      </c>
-      <c r="E14">
-        <v>1670.41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="68">
-        <v>0.8847222222222223</v>
-      </c>
-      <c r="E15">
-        <v>2333.04</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="68">
-        <v>0.88611111111111107</v>
-      </c>
-      <c r="E16">
-        <v>1798.79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="68">
-        <v>0.88750000000000007</v>
-      </c>
-      <c r="E17">
-        <v>1321.49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="68">
-        <v>0.8881944444444444</v>
-      </c>
-      <c r="E18">
-        <v>1644.36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="68">
-        <v>0.88958333333333339</v>
-      </c>
-      <c r="E19">
-        <v>1327.65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="68">
-        <v>0.89097222222222217</v>
-      </c>
-      <c r="E20">
-        <v>1569.41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="68">
-        <v>0.89166666666666661</v>
-      </c>
-      <c r="E21">
-        <v>2825.98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="68">
-        <v>0.8930555555555556</v>
-      </c>
-      <c r="E22">
-        <v>1379.75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="68">
-        <v>0.89513888888888893</v>
-      </c>
-      <c r="E24">
-        <v>2426.37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="68">
-        <v>0.8965277777777777</v>
-      </c>
-      <c r="E25">
-        <v>1338.72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="68">
-        <v>0.8979166666666667</v>
-      </c>
-      <c r="E26">
-        <v>1678.06</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="68">
-        <v>0.89861111111111114</v>
-      </c>
-      <c r="E27">
-        <v>1222.3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="68">
-        <v>0.90208333333333324</v>
-      </c>
-      <c r="E29">
-        <v>1167.4100000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="68">
-        <v>0.90208333333333324</v>
-      </c>
-      <c r="E30">
-        <v>2643.27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="68">
-        <v>0.90347222222222223</v>
-      </c>
-      <c r="E31">
-        <v>1706.59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="68">
-        <v>0.90486111111111101</v>
-      </c>
-      <c r="E32">
-        <v>1210.6300000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="68">
-        <v>0.90555555555555556</v>
-      </c>
-      <c r="E33">
-        <v>833.41499999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="68">
-        <v>0.90694444444444444</v>
-      </c>
-      <c r="E34">
-        <v>1037.95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="68">
-        <v>0.90833333333333333</v>
-      </c>
-      <c r="E35">
-        <v>1279.22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>36</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="68">
-        <v>0.90972222222222221</v>
-      </c>
-      <c r="E36">
-        <v>1220.81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="68">
-        <v>0.91041666666666676</v>
-      </c>
-      <c r="E37">
-        <v>1746.34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="68">
-        <v>0.91180555555555554</v>
-      </c>
-      <c r="E38">
-        <v>3474.18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="68">
-        <v>0.91249999999999998</v>
-      </c>
-      <c r="E40">
-        <v>1188.3399999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>42</v>
-      </c>
-      <c r="B42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="68">
-        <v>0.9194444444444444</v>
-      </c>
-      <c r="E42">
-        <v>3256.97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>43</v>
-      </c>
-      <c r="B43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="68">
-        <v>0.92083333333333339</v>
-      </c>
-      <c r="E43">
-        <v>2848.14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="68">
-        <v>0.92222222222222217</v>
-      </c>
-      <c r="E44">
-        <v>2483.09</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>45</v>
-      </c>
-      <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="68">
-        <v>0.92291666666666661</v>
-      </c>
-      <c r="E45">
-        <v>1144.73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>46</v>
-      </c>
-      <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="68">
-        <v>0.9243055555555556</v>
-      </c>
-      <c r="E46">
-        <v>1250.8800000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="68">
-        <v>0.92569444444444438</v>
-      </c>
-      <c r="E47">
-        <v>1578.94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" t="s">
-        <v>67</v>
-      </c>
-      <c r="D48" s="68">
-        <v>0.92638888888888893</v>
-      </c>
-      <c r="E48">
-        <v>1505.33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="68">
-        <v>0.9277777777777777</v>
-      </c>
-      <c r="E49">
-        <v>986.79100000000005</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>50</v>
-      </c>
-      <c r="B50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="68">
-        <v>0.92847222222222225</v>
-      </c>
-      <c r="E50">
-        <v>1385.28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="68">
-        <v>0.92986111111111114</v>
-      </c>
-      <c r="E51">
-        <v>1180.6500000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="68">
-        <v>0.93125000000000002</v>
-      </c>
-      <c r="E52">
-        <v>2103.15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>53</v>
-      </c>
-      <c r="B53" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" t="s">
-        <v>67</v>
-      </c>
-      <c r="D53" s="68">
-        <v>0.93263888888888891</v>
-      </c>
-      <c r="E53">
-        <v>2834.3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>54</v>
-      </c>
-      <c r="B54" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="68">
-        <v>0.93333333333333324</v>
-      </c>
-      <c r="E54">
-        <v>2666.23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>55</v>
-      </c>
-      <c r="B55" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" t="s">
-        <v>67</v>
-      </c>
-      <c r="D55" s="68">
-        <v>0.93472222222222223</v>
-      </c>
-      <c r="E55">
-        <v>2044.38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>56</v>
-      </c>
-      <c r="B56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="68">
-        <v>0.93611111111111101</v>
-      </c>
-      <c r="E56">
-        <v>1809.44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>57</v>
-      </c>
-      <c r="B57" t="s">
-        <v>61</v>
-      </c>
-      <c r="C57" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="68">
-        <v>0.93680555555555556</v>
-      </c>
-      <c r="E57">
-        <v>1892.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>58</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="68">
-        <v>0.93819444444444444</v>
-      </c>
-      <c r="E58">
-        <v>2167.96</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>59</v>
-      </c>
-      <c r="B59" t="s">
-        <v>61</v>
-      </c>
-      <c r="C59" t="s">
-        <v>67</v>
-      </c>
-      <c r="D59" s="68">
-        <v>0.93958333333333333</v>
-      </c>
-      <c r="E59">
-        <v>1530.38</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>60</v>
-      </c>
-      <c r="B60" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" t="s">
-        <v>67</v>
-      </c>
-      <c r="D60" s="68">
-        <v>0.94027777777777777</v>
-      </c>
-      <c r="E60">
-        <v>6760.81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>61</v>
-      </c>
-      <c r="B61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" t="s">
-        <v>67</v>
-      </c>
-      <c r="D61" s="68">
-        <v>0.94166666666666676</v>
-      </c>
-      <c r="E61">
-        <v>1893.57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>62</v>
-      </c>
-      <c r="B62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" t="s">
-        <v>67</v>
-      </c>
-      <c r="D62" s="68">
-        <v>0.94305555555555554</v>
-      </c>
-      <c r="E62">
-        <v>1420.11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>63</v>
-      </c>
-      <c r="B63" t="s">
-        <v>61</v>
-      </c>
-      <c r="C63" t="s">
-        <v>67</v>
-      </c>
-      <c r="D63" s="68">
-        <v>0.94374999999999998</v>
-      </c>
-      <c r="E63">
-        <v>1566.81</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>64</v>
-      </c>
-      <c r="B64" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" t="s">
-        <v>67</v>
-      </c>
-      <c r="D64" s="68">
-        <v>0.94513888888888886</v>
-      </c>
-      <c r="E64">
-        <v>2919.93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>65</v>
-      </c>
-      <c r="B65" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" t="s">
-        <v>67</v>
-      </c>
-      <c r="D65" s="68">
-        <v>0.9458333333333333</v>
-      </c>
-      <c r="E65">
-        <v>1989.72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>66</v>
-      </c>
-      <c r="B66" t="s">
-        <v>61</v>
-      </c>
-      <c r="C66" t="s">
-        <v>67</v>
-      </c>
-      <c r="D66" s="68">
-        <v>0.9472222222222223</v>
-      </c>
-      <c r="E66">
-        <v>2421.12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>67</v>
-      </c>
-      <c r="B67" t="s">
-        <v>61</v>
-      </c>
-      <c r="C67" t="s">
-        <v>67</v>
-      </c>
-      <c r="D67" s="68">
-        <v>0.94861111111111107</v>
-      </c>
-      <c r="E67">
-        <v>1088.8599999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>68</v>
-      </c>
-      <c r="B68" t="s">
-        <v>61</v>
-      </c>
-      <c r="C68" t="s">
-        <v>67</v>
-      </c>
-      <c r="D68" s="68">
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="E68">
-        <v>2715.15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>69</v>
-      </c>
-      <c r="B69" t="s">
-        <v>61</v>
-      </c>
-      <c r="C69" t="s">
-        <v>67</v>
-      </c>
-      <c r="D69" s="68">
-        <v>0.9506944444444444</v>
-      </c>
-      <c r="E69">
-        <v>1690.46</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>70</v>
-      </c>
-      <c r="B70" t="s">
-        <v>61</v>
-      </c>
-      <c r="C70" t="s">
-        <v>67</v>
-      </c>
-      <c r="D70" s="68">
-        <v>0.95208333333333339</v>
-      </c>
-      <c r="E70">
-        <v>2796.21</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>71</v>
-      </c>
-      <c r="B71" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" t="s">
-        <v>67</v>
-      </c>
-      <c r="D71" s="68">
-        <v>0.95277777777777783</v>
-      </c>
-      <c r="E71">
-        <v>2051.7399999999998</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>72</v>
-      </c>
-      <c r="B72" t="s">
-        <v>61</v>
-      </c>
-      <c r="C72" t="s">
-        <v>67</v>
-      </c>
-      <c r="D72" s="68">
-        <v>0.95416666666666661</v>
-      </c>
-      <c r="E72">
-        <v>2521.66</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>73</v>
-      </c>
-      <c r="B73" t="s">
-        <v>61</v>
-      </c>
-      <c r="C73" t="s">
-        <v>67</v>
-      </c>
-      <c r="D73" s="68">
-        <v>0.9555555555555556</v>
-      </c>
-      <c r="E73">
-        <v>1735.03</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>74</v>
-      </c>
-      <c r="B74" t="s">
-        <v>61</v>
-      </c>
-      <c r="C74" t="s">
-        <v>67</v>
-      </c>
-      <c r="D74" s="68">
-        <v>0.95624999999999993</v>
-      </c>
-      <c r="E74">
-        <v>1010.37</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>75</v>
-      </c>
-      <c r="B75" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" t="s">
-        <v>67</v>
-      </c>
-      <c r="D75" s="68">
-        <v>0.95763888888888893</v>
-      </c>
-      <c r="E75">
-        <v>1736.02</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>76</v>
-      </c>
-      <c r="B76" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" t="s">
-        <v>67</v>
-      </c>
-      <c r="D76" s="68">
-        <v>0.9590277777777777</v>
-      </c>
-      <c r="E76">
-        <v>1533.68</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>77</v>
-      </c>
-      <c r="B77" t="s">
-        <v>61</v>
-      </c>
-      <c r="C77" t="s">
-        <v>67</v>
-      </c>
-      <c r="D77" s="68">
-        <v>0.95972222222222225</v>
-      </c>
-      <c r="E77">
-        <v>2119.84</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>78</v>
-      </c>
-      <c r="B78" t="s">
-        <v>61</v>
-      </c>
-      <c r="C78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D78" s="68">
-        <v>0.96111111111111114</v>
-      </c>
-      <c r="E78">
-        <v>2422.75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>79</v>
-      </c>
-      <c r="B79" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" t="s">
-        <v>67</v>
-      </c>
-      <c r="D79" s="68">
-        <v>0.96250000000000002</v>
-      </c>
-      <c r="E79">
-        <v>2379.73</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>80</v>
-      </c>
-      <c r="B80" t="s">
-        <v>61</v>
-      </c>
-      <c r="C80" t="s">
-        <v>67</v>
-      </c>
-      <c r="D80" s="68">
-        <v>0.96319444444444446</v>
-      </c>
-      <c r="E80">
-        <v>1289.8499999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>81</v>
-      </c>
-      <c r="B81" t="s">
-        <v>61</v>
-      </c>
-      <c r="C81" t="s">
-        <v>67</v>
-      </c>
-      <c r="D81" s="68">
-        <v>0.96458333333333324</v>
-      </c>
-      <c r="E81">
-        <v>1336.74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>82</v>
-      </c>
-      <c r="B82" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" t="s">
-        <v>67</v>
-      </c>
-      <c r="D82" s="68">
-        <v>0.96597222222222223</v>
-      </c>
-      <c r="E82">
-        <v>1500.93</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>83</v>
-      </c>
-      <c r="B83" t="s">
-        <v>61</v>
-      </c>
-      <c r="C83" t="s">
-        <v>67</v>
-      </c>
-      <c r="D83" s="68">
-        <v>0.96666666666666667</v>
-      </c>
-      <c r="E83">
-        <v>2145.6999999999998</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>84</v>
-      </c>
-      <c r="B84" t="s">
-        <v>61</v>
-      </c>
-      <c r="C84" t="s">
-        <v>67</v>
-      </c>
-      <c r="D84" s="68">
-        <v>0.96875</v>
-      </c>
-      <c r="E84">
-        <v>1385.37</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>86</v>
-      </c>
-      <c r="B86" t="s">
-        <v>61</v>
-      </c>
-      <c r="C86" t="s">
-        <v>67</v>
-      </c>
-      <c r="D86" s="68">
-        <v>0.97083333333333333</v>
-      </c>
-      <c r="E86">
-        <v>3027.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>87</v>
-      </c>
-      <c r="B87" t="s">
-        <v>61</v>
-      </c>
-      <c r="C87" t="s">
-        <v>67</v>
-      </c>
-      <c r="D87" s="68">
-        <v>0.97152777777777777</v>
-      </c>
-      <c r="E87">
-        <v>1019.59</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>88</v>
-      </c>
-      <c r="B88" t="s">
-        <v>61</v>
-      </c>
-      <c r="C88" t="s">
-        <v>67</v>
-      </c>
-      <c r="D88" s="68">
-        <v>0.97291666666666676</v>
-      </c>
-      <c r="E88">
-        <v>2959.24</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>89</v>
-      </c>
-      <c r="B89" t="s">
-        <v>61</v>
-      </c>
-      <c r="C89" t="s">
-        <v>67</v>
-      </c>
-      <c r="D89" s="68">
-        <v>0.97361111111111109</v>
-      </c>
-      <c r="E89">
-        <v>415.39800000000002</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>90</v>
-      </c>
-      <c r="B90" t="s">
-        <v>61</v>
-      </c>
-      <c r="C90" t="s">
-        <v>67</v>
-      </c>
-      <c r="D90" s="68">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="E90">
-        <v>4008.79</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>91</v>
-      </c>
-      <c r="B91" t="s">
-        <v>61</v>
-      </c>
-      <c r="C91" t="s">
-        <v>67</v>
-      </c>
-      <c r="D91" s="68">
-        <v>0.97638888888888886</v>
-      </c>
-      <c r="E91">
-        <v>2202.6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>92</v>
-      </c>
-      <c r="B92" t="s">
-        <v>61</v>
-      </c>
-      <c r="C92" t="s">
-        <v>67</v>
-      </c>
-      <c r="D92" s="68">
-        <v>0.97777777777777775</v>
-      </c>
-      <c r="E92">
-        <v>2022.86</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>93</v>
-      </c>
-      <c r="B93" t="s">
-        <v>61</v>
-      </c>
-      <c r="C93" t="s">
-        <v>67</v>
-      </c>
-      <c r="D93" s="68">
-        <v>0.9784722222222223</v>
-      </c>
-      <c r="E93">
-        <v>1407.75</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>94</v>
-      </c>
-      <c r="B94" t="s">
-        <v>61</v>
-      </c>
-      <c r="C94" t="s">
-        <v>67</v>
-      </c>
-      <c r="D94" s="68">
-        <v>0.97986111111111107</v>
-      </c>
-      <c r="E94">
-        <v>2469.14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>95</v>
-      </c>
-      <c r="B95" t="s">
-        <v>61</v>
-      </c>
-      <c r="C95" t="s">
-        <v>67</v>
-      </c>
-      <c r="D95" s="68">
-        <v>0.98125000000000007</v>
-      </c>
-      <c r="E95">
-        <v>2762.21</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>96</v>
-      </c>
-      <c r="B96" t="s">
-        <v>61</v>
-      </c>
-      <c r="C96" t="s">
-        <v>67</v>
-      </c>
-      <c r="D96" s="68">
-        <v>0.9819444444444444</v>
-      </c>
-      <c r="E96">
-        <v>1576.98</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>97</v>
-      </c>
-      <c r="B97" t="s">
-        <v>61</v>
-      </c>
-      <c r="C97" t="s">
-        <v>67</v>
-      </c>
-      <c r="D97" s="68">
-        <v>0.98333333333333339</v>
-      </c>
-      <c r="E97">
-        <v>2039.7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>98</v>
-      </c>
-      <c r="B98" t="s">
-        <v>61</v>
-      </c>
-      <c r="C98" t="s">
-        <v>67</v>
-      </c>
-      <c r="D98" s="68">
-        <v>0.98472222222222217</v>
-      </c>
-      <c r="E98">
-        <v>1446.6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>99</v>
-      </c>
-      <c r="B99" t="s">
-        <v>61</v>
-      </c>
-      <c r="C99" t="s">
-        <v>67</v>
-      </c>
-      <c r="D99" s="68">
-        <v>0.98541666666666661</v>
-      </c>
-      <c r="E99">
-        <v>2326.4499999999998</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>100</v>
-      </c>
-      <c r="B100" t="s">
-        <v>61</v>
-      </c>
-      <c r="C100" t="s">
-        <v>67</v>
-      </c>
-      <c r="D100" s="68">
-        <v>0.9868055555555556</v>
-      </c>
-      <c r="E100">
-        <v>1743.42</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>101</v>
-      </c>
-      <c r="B101" t="s">
-        <v>61</v>
-      </c>
-      <c r="C101" t="s">
-        <v>67</v>
-      </c>
-      <c r="D101" s="68">
-        <v>0.98819444444444438</v>
-      </c>
-      <c r="E101">
-        <v>3221.66</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>102</v>
-      </c>
-      <c r="B102" t="s">
-        <v>61</v>
-      </c>
-      <c r="C102" t="s">
-        <v>67</v>
-      </c>
-      <c r="D102" s="68">
-        <v>0.98888888888888893</v>
-      </c>
-      <c r="E102">
-        <v>381.05599999999998</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>103</v>
-      </c>
-      <c r="B103" t="s">
-        <v>61</v>
-      </c>
-      <c r="C103" t="s">
-        <v>67</v>
-      </c>
-      <c r="D103" s="68">
-        <v>0.9902777777777777</v>
-      </c>
-      <c r="E103">
-        <v>2586.61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -18223,6 +16512,31 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DLCPolicyLabelClientValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">{_UIVersionString}</DLCPolicyLabelClientValue>
+    <_dlc_BarcodeImage xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">iVBORw0KGgoAAAANSUhEUgAAAYIAAABtCAYAAACsn2ZqAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAABp9SURBVHhe7ZvBihzbsiz3///0eeiBgeGE54qsTA0uSgMfWLt3aA2aqpH++9/Hx8fHxz/N90Xw8fHx8Y/zfRF8fHx8/ON8XwQfHx8f/zjfF8HHx8fHP873RfDx8fHxj/P6F8F///33/zORHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef/ix8fHx8f/Kb4vgo+Pj49/nO+L4OPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+/irtP7/wH2OmwNQRc9XBWxu46k93snfMVffx8SbfX9fHX+XuB5j3m9+dNvmztzamdb/+W8nmzsfHW3x/WR9/hT8fWmRLbk+/e9XTbTZX5OaPk+Tqnrur3Yknv/vx0fj+qj7+Knc+uHJ7+t2rnm6zuaJtpp9v/63Nv9t48rsfH43vr+rjr7L94Jp2f36WSU4/m3q46v7wy+9OP8+f/fHMljvbj48t31/Vx19l+8H1ZPfnZ46Z9jB17U5yuru9A5vd9tbHx12+v6yPv8rf+IDzfvrd/FnbTD83V33r2r+14Zd/7+PjDb6/ro+/yuYD7O6HHPs7H5x/3OFnJ9pm+vnVvbf/rY+PN/n+wj7+KqcPsV8+5Pidq9/d3H2ymX7+N96z+b2Pj6d8f2Uff5XTB9kvH3T8ztXvvvXvtt308yfv+UNuNr/z8fEG31/ax1/lyYfj1G8+LN+4+4erO63b3Pl18/Hxt/j+2j7+Cn8+yDLJ9LPkdOMPp82ph80uN9Pu1P/htMne+fh4m++v6uPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+Pj4+/nG+L4KPj4+Pf5r//e//AYQWEYJwHQKsAAAAAElFTkSuQmCC</_dlc_BarcodeImage>
+    <DLCPolicyLabelLock xmlns="e2656bbd-0e15-4aa0-af00-25744e385561" xsi:nil="true"/>
+    <_dlc_BarcodeValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">1758931852</_dlc_BarcodeValue>
+    <_dlc_BarcodePreview xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">
+      <Url>https://surgiceye.sharepoint.com/dev/_layouts/15/barcodeimagefromitem.aspx?ID=419111&amp;list=e2656bbd-0e15-4aa0-af00-25744e385561</Url>
+      <Description>Barcode: 1758931852</Description>
+    </_dlc_BarcodePreview>
+    <DLCPolicyLabelValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">0.3</DLCPolicyLabelValue>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="SurgicEye WordTemplate" ma:contentTypeID="0x01010074A3F29CB79E8A41A92E73E19AE321CB00098C261D3F46DB49AEA371869FEC377C" ma:contentTypeVersion="17" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="d27efd9bfa2cf0dc081f61d6777772ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e2656bbd-0e15-4aa0-af00-25744e385561" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53fececc5845ce19907e3af2573e5d2e" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18398,31 +16712,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DLCPolicyLabelClientValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">{_UIVersionString}</DLCPolicyLabelClientValue>
-    <_dlc_BarcodeImage xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">iVBORw0KGgoAAAANSUhEUgAAAYIAAABtCAYAAACsn2ZqAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAABp9SURBVHhe7ZvBihzbsiz3///0eeiBgeGE54qsTA0uSgMfWLt3aA2aqpH++9/Hx8fHxz/N90Xw8fHx8Y/zfRF8fHx8/ON8XwQfHx8f/zjfF8HHx8fHP873RfDx8fHxj/P6F8F///33/zORHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef/ix8fHx8f/Kb4vgo+Pj49/nO+L4OPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+/irtP7/wH2OmwNQRc9XBWxu46k93snfMVffx8SbfX9fHX+XuB5j3m9+dNvmztzamdb/+W8nmzsfHW3x/WR9/hT8fWmRLbk+/e9XTbTZX5OaPk+Tqnrur3Yknv/vx0fj+qj7+Knc+uHJ7+t2rnm6zuaJtpp9v/63Nv9t48rsfH43vr+rjr7L94Jp2f36WSU4/m3q46v7wy+9OP8+f/fHMljvbj48t31/Vx19l+8H1ZPfnZ46Z9jB17U5yuru9A5vd9tbHx12+v6yPv8rf+IDzfvrd/FnbTD83V33r2r+14Zd/7+PjDb6/ro+/yuYD7O6HHPs7H5x/3OFnJ9pm+vnVvbf/rY+PN/n+wj7+KqcPsV8+5Pidq9/d3H2ymX7+N96z+b2Pj6d8f2Uff5XTB9kvH3T8ztXvvvXvtt308yfv+UNuNr/z8fEG31/ax1/lyYfj1G8+LN+4+4erO63b3Pl18/Hxt/j+2j7+Cn8+yDLJ9LPkdOMPp82ph80uN9Pu1P/htMne+fh4m++v6uPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+Pj4+/nG+L4KPj4+Pf5r//e//AYQWEYJwHQKsAAAAAElFTkSuQmCC</_dlc_BarcodeImage>
-    <DLCPolicyLabelLock xmlns="e2656bbd-0e15-4aa0-af00-25744e385561" xsi:nil="true"/>
-    <_dlc_BarcodeValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">1758931852</_dlc_BarcodeValue>
-    <_dlc_BarcodePreview xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">
-      <Url>https://surgiceye.sharepoint.com/dev/_layouts/15/barcodeimagefromitem.aspx?ID=419111&amp;list=e2656bbd-0e15-4aa0-af00-25744e385561</Url>
-      <Description>Barcode: 1758931852</Description>
-    </_dlc_BarcodePreview>
-    <DLCPolicyLabelValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">0.3</DLCPolicyLabelValue>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A933A0-2E29-4D82-A4A8-6FECA8CC0598}">
   <ds:schemaRefs>
@@ -18432,20 +16721,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8953B42-7F0B-4652-8904-3F0A580F556B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3611D48C-6B4F-4CD9-8579-A2A41CE94ADA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e2656bbd-0e15-4aa0-af00-25744e385561"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18468,9 +16746,20 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3611D48C-6B4F-4CD9-8579-A2A41CE94ADA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8953B42-7F0B-4652-8904-3F0A580F556B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e2656bbd-0e15-4aa0-af00-25744e385561"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>